<commit_message>
Add File Deskripsi Game & Update README.md
</commit_message>
<xml_diff>
--- a/Kunci Jawaban.xlsx
+++ b/Kunci Jawaban.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Git\kbb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KBB Release\Game Android Kuis Bolak-Balik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B31BFAB-38B4-46CB-880B-80C3220691A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F898B9F-59A0-432B-8B74-400CBB002159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B84D0AA6-B0E1-4A2D-A1F7-81F6BE7F993D}"/>
   </bookViews>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>POLOIJTSKY</t>
-  </si>
-  <si>
-    <t>UKNGPARKRML</t>
   </si>
   <si>
     <t>DDYCOBUZER</t>
@@ -161,12 +158,6 @@
     </r>
   </si>
   <si>
-    <t>KUIS BOLAK-BALIK (Cobalah Tebak, Ayooo Doooong!)</t>
-  </si>
-  <si>
-    <t>Copyright © 2021 BaCod Studio (Bagus Coding Studio)</t>
-  </si>
-  <si>
     <t>PREMAN</t>
   </si>
   <si>
@@ -176,14 +167,35 @@
     <t>https://github.com/baguspangestu/kbb</t>
   </si>
   <si>
-    <t>Project Tersedia di Github:</t>
+    <t>Project Juga Tersedia di Github:</t>
+  </si>
+  <si>
+    <r>
+      <t>UKNGPARKR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ML</t>
+    </r>
+  </si>
+  <si>
+    <t>KUIS BOLAK-BALIK</t>
+  </si>
+  <si>
+    <t>© 2021 BaCod Studio (www.bacod-studio.web.app)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +261,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +342,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -349,10 +368,19 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -361,10 +389,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -687,10 +712,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7632F04C-EBAC-4871-AD86-2E95247BBC11}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B3:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,41 +730,41 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
+      <c r="B3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="I5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -750,19 +778,19 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -773,22 +801,22 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -802,19 +830,19 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -824,23 +852,23 @@
       <c r="C9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -851,22 +879,22 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -877,51 +905,51 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="B13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="B15" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -932,38 +960,38 @@
       <c r="I16" s="13"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="B18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="B19" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -977,8 +1005,9 @@
   <hyperlinks>
     <hyperlink ref="B16:I16" r:id="rId1" display="Tersedia di Github: https://github.com/baguspangestu/kbb" xr:uid="{FE6F8D21-C026-4B5A-9CFD-35866DDE6A1A}"/>
     <hyperlink ref="B16" r:id="rId2" xr:uid="{DF63D1D0-AD21-4E86-9E6E-93786EB0C186}"/>
+    <hyperlink ref="B19:I19" r:id="rId3" display="© 2021 BaCod Studio (Bagus Coding Studio)" xr:uid="{4FE0E457-72F4-4364-B7CC-E7A7AC821385}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="82" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Deskripsi Game, & Kunci Jawaban
</commit_message>
<xml_diff>
--- a/Kunci Jawaban.xlsx
+++ b/Kunci Jawaban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KBB Release\Game Android Kuis Bolak-Balik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F898B9F-59A0-432B-8B74-400CBB002159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F69753-A93F-4D28-BE0B-4F4E371A1C7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B84D0AA6-B0E1-4A2D-A1F7-81F6BE7F993D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>BULUTANGKIS</t>
   </si>
@@ -133,12 +133,42 @@
   </si>
   <si>
     <t>JEBAKAN 4</t>
+  </si>
+  <si>
+    <t>PREMAN</t>
+  </si>
+  <si>
+    <t>https://github.com/baguspangestu/kbb</t>
+  </si>
+  <si>
+    <t>Project Juga Tersedia di Github:</t>
+  </si>
+  <si>
+    <t>KUIS BOLAK-BALIK</t>
+  </si>
+  <si>
+    <t>© 2021 AMIK DCC PRINGSEWU</t>
+  </si>
+  <si>
+    <r>
+      <t>UKNGPARKR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ML</t>
+    </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -148,7 +178,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -157,45 +187,12 @@
       <t xml:space="preserve"> berfungsi untuk menambah karakter supaya menjadi 16 karakter  ketika ditambahkan dg jawaban (karena tombol keyboard di dalam game dibuat 16 karakter) dan juga dibikin supaya nyambung dengan jebakan, jadi untuk menambah karakter tambahan juga tidak asal-asalan.</t>
     </r>
   </si>
-  <si>
-    <t>PREMAN</t>
-  </si>
-  <si>
-    <t>AMIK DCC PRINGSEWU</t>
-  </si>
-  <si>
-    <t>https://github.com/baguspangestu/kbb</t>
-  </si>
-  <si>
-    <t>Project Juga Tersedia di Github:</t>
-  </si>
-  <si>
-    <r>
-      <t>UKNGPARKR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ML</t>
-    </r>
-  </si>
-  <si>
-    <t>KUIS BOLAK-BALIK</t>
-  </si>
-  <si>
-    <t>© 2021 BaCod Studio (www.bacod-studio.web.app)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,31 +208,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -249,15 +223,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -266,8 +231,54 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,61 +346,56 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -715,10 +721,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B3:I19"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,227 +735,255 @@
     <col min="6" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B3" s="14" t="s">
+    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -959,55 +993,53 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+    <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B13:I13"/>
+  <mergeCells count="5">
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B17:I17"/>
     <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B15:I15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B16:I16" r:id="rId1" display="Tersedia di Github: https://github.com/baguspangestu/kbb" xr:uid="{FE6F8D21-C026-4B5A-9CFD-35866DDE6A1A}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{DF63D1D0-AD21-4E86-9E6E-93786EB0C186}"/>
-    <hyperlink ref="B19:I19" r:id="rId3" display="© 2021 BaCod Studio (Bagus Coding Studio)" xr:uid="{4FE0E457-72F4-4364-B7CC-E7A7AC821385}"/>
+    <hyperlink ref="B17:I17" r:id="rId1" display="Tersedia di Github: https://github.com/baguspangestu/kbb" xr:uid="{FE6F8D21-C026-4B5A-9CFD-35866DDE6A1A}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{DF63D1D0-AD21-4E86-9E6E-93786EB0C186}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="82" orientation="landscape" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="82" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>